<commit_message>
Re evaluacion de rubrica entrega tardia de estudiante a evaluar
</commit_message>
<xml_diff>
--- a/RúbricaDeEvaluación.xlsx
+++ b/RúbricaDeEvaluación.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolai Bermudez V\Desktop\Nico nico ni\SISTEMAS\9 Semestre\AREP\AREP-LAB-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B345C9F-5523-43B4-9903-9D07CD30E642}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC45CC69-DDE3-40D8-92B6-5566AE4D5D0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="20730" windowHeight="11835" xr2:uid="{30389B9F-C7D3-A542-9567-157FC0B6A65B}"/>
+    <workbookView xWindow="-1590" yWindow="2520" windowWidth="20730" windowHeight="11835" xr2:uid="{30389B9F-C7D3-A542-9567-157FC0B6A65B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Diseño</t>
   </si>
@@ -177,7 +168,10 @@
     <t>PULIDO RINCON JAIRO EDUARDO</t>
   </si>
   <si>
-    <t>No encontre algun repositorio</t>
+    <t>https://github.com/Killersys/AREP-LAB3</t>
+  </si>
+  <si>
+    <t>Entrega tardia debido a que subio repositorio el 24 de febrero</t>
   </si>
 </sst>
 </file>
@@ -305,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -341,6 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -658,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7759D1B1-2861-2D40-A5C1-6BA06F856130}">
   <dimension ref="A3:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -702,7 +697,9 @@
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="C6" s="13"/>
       <c r="D6" s="1"/>
     </row>
@@ -711,7 +708,7 @@
         <v>38</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="1"/>
@@ -760,7 +757,7 @@
       </c>
       <c r="C13" s="7">
         <f>SUM(C14:C20)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -782,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -793,7 +790,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -804,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -815,7 +812,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,7 +834,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -855,7 +852,7 @@
       </c>
       <c r="C22" s="7">
         <f>SUM(C23:C32)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -866,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -877,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,7 +896,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -921,7 +918,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,7 +929,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -943,7 +940,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,7 +951,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -965,15 +962,15 @@
         <v>3</v>
       </c>
       <c r="C32" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>0</v>
       </c>
@@ -983,10 +980,10 @@
       </c>
       <c r="C34" s="7">
         <f>SUM(C35:C38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -994,10 +991,10 @@
         <v>4</v>
       </c>
       <c r="C35" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -1005,10 +1002,10 @@
         <v>4</v>
       </c>
       <c r="C36" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>9</v>
       </c>
@@ -1016,10 +1013,10 @@
         <v>4</v>
       </c>
       <c r="C37" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>32</v>
       </c>
@@ -1027,15 +1024,15 @@
         <v>4</v>
       </c>
       <c r="C38" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>20</v>
       </c>
@@ -1045,10 +1042,10 @@
       </c>
       <c r="C40" s="7">
         <f>SUM(C41:C45)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>10</v>
       </c>
@@ -1056,10 +1053,10 @@
         <v>3</v>
       </c>
       <c r="C41" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>11</v>
       </c>
@@ -1068,10 +1065,11 @@
         <v>6</v>
       </c>
       <c r="C42" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D42" s="17"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>12</v>
       </c>
@@ -1079,10 +1077,10 @@
         <v>3</v>
       </c>
       <c r="C43" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>13</v>
       </c>
@@ -1090,10 +1088,10 @@
         <v>3</v>
       </c>
       <c r="C44" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>22</v>
       </c>
@@ -1101,15 +1099,15 @@
         <v>3</v>
       </c>
       <c r="C45" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="6"/>
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>1</v>
       </c>
@@ -1119,10 +1117,10 @@
       </c>
       <c r="C47" s="7">
         <f>SUM(C48:C52)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>14</v>
       </c>
@@ -1130,7 +1128,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,7 +1139,7 @@
         <v>3</v>
       </c>
       <c r="C49" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1152,7 +1150,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1163,7 +1161,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1174,7 +1172,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1192,7 +1190,7 @@
       </c>
       <c r="C54" s="7">
         <f>SUM(C47,C40,C34,C22,C13)</f>
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1205,7 +1203,7 @@
       </c>
       <c r="C55" s="7">
         <f>C54/$B$54*5</f>
-        <v>0</v>
+        <v>4.7023809523809526</v>
       </c>
     </row>
   </sheetData>
@@ -1217,7 +1215,10 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B7:C9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{E4E0A617-4874-4674-9276-01F7BE872D00}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>